<commit_message>
Added changable column names
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ET\toXML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A89B2FC-AFF7-4F3E-B5BE-864C21F57598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF54F5F-7C41-4EAE-9E26-8857F6E40F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>A01</t>
   </si>
@@ -66,19 +66,22 @@
     <t>Rozdzielczość</t>
   </si>
   <si>
-    <t>WYTW1</t>
-  </si>
-  <si>
-    <t>WYTW2</t>
-  </si>
-  <si>
-    <t>WYTW3</t>
-  </si>
-  <si>
     <t>MRID1</t>
   </si>
   <si>
     <t>MRID2</t>
+  </si>
+  <si>
+    <t>Opis</t>
+  </si>
+  <si>
+    <t>WytwPierwszy</t>
+  </si>
+  <si>
+    <t>WytwDrugi</t>
+  </si>
+  <si>
+    <t>WytwTrzeci</t>
   </si>
 </sst>
 </file>
@@ -400,25 +403,29 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -496,13 +503,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>